<commit_message>
single choice field implemented and omitempty added in json
</commit_message>
<xml_diff>
--- a/testdata/m&e.xlsx
+++ b/testdata/m&e.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>type</t>
   </si>
@@ -85,6 +85,33 @@
   </si>
   <si>
     <t>markets_monitoring</t>
+  </si>
+  <si>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>_1</t>
+  </si>
+  <si>
+    <t>Implementation period</t>
+  </si>
+  <si>
+    <t>end group</t>
+  </si>
+  <si>
+    <t>_2</t>
+  </si>
+  <si>
+    <t>Monitoring visits</t>
+  </si>
+  <si>
+    <t>select_one IMPLEMENTATION_PERIOD</t>
+  </si>
+  <si>
+    <t>_1_100</t>
+  </si>
+  <si>
+    <t>Please select one of the following</t>
   </si>
 </sst>
 </file>
@@ -403,13 +430,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -422,8 +453,52 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -431,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
refactoring of xls2ajf function
</commit_message>
<xml_diff>
--- a/testdata/m&e.xlsx
+++ b/testdata/m&e.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>type</t>
   </si>
@@ -112,6 +112,33 @@
   </si>
   <si>
     <t>Please select one of the following</t>
+  </si>
+  <si>
+    <t>select_one MONITORING_VISITS</t>
+  </si>
+  <si>
+    <t>_2_200</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>_2_202</t>
+  </si>
+  <si>
+    <t>Name of monitoring visitor</t>
+  </si>
+  <si>
+    <t>_2_203</t>
+  </si>
+  <si>
+    <t>Position of monitoring visitor</t>
+  </si>
+  <si>
+    <t>_2_204</t>
+  </si>
+  <si>
+    <t>Main conclusions of the monitoring visit</t>
   </si>
 </sst>
 </file>
@@ -430,16 +457,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -493,6 +520,50 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
id assignment fixed again and date field added
</commit_message>
<xml_diff>
--- a/testdata/m&e.xlsx
+++ b/testdata/m&e.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>type</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Main conclusions of the monitoring visit</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>_2_201</t>
+  </si>
+  <si>
+    <t>Date of the monitoring visit</t>
   </si>
 </sst>
 </file>
@@ -457,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,13 +540,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -545,10 +554,10 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -556,14 +565,25 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
required column implemented as validation.notEmpty
</commit_message>
<xml_diff>
--- a/testdata/m&e.xlsx
+++ b/testdata/m&e.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>type</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Date of the monitoring visit</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -466,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +484,7 @@
     <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +494,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -500,7 +509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -510,13 +519,16 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -527,7 +539,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -537,8 +549,11 @@
       <c r="C8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -548,8 +563,11 @@
       <c r="C9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -559,8 +577,11 @@
       <c r="C10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -570,8 +591,11 @@
       <c r="C11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -581,8 +605,11 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
fixed typo: list_name -> 'list name'. XlsForm struct changed to accomodate future features
</commit_message>
<xml_diff>
--- a/testdata/m&e.xlsx
+++ b/testdata/m&e.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robza\go\src\github.com\pinkgopher\xls2ajf\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robza\go\src\bitbucket.org\gnucoop\xls2ajf\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>label</t>
   </si>
   <si>
-    <t>list_name</t>
-  </si>
-  <si>
     <t>IMPLEMENTATION_PERIOD</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>list name</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -495,123 +495,123 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -624,9 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -637,7 +635,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -648,79 +646,79 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>